<commit_message>
vault backup: 2022-09-07 12:44:50
</commit_message>
<xml_diff>
--- a/情感识别结果数据.xlsx
+++ b/情感识别结果数据.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC6746D-98B1-4137-B8CE-60FF08F0CCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A608E1A2-4AD5-4B13-923A-3931CDCAA4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B194B2CE-EAD3-430D-A074-ECB720BDCFAC}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{B194B2CE-EAD3-430D-A074-ECB720BDCFAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1246,6 +1246,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A1:A3"/>
@@ -1253,12 +1259,6 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H1:P1"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>